<commit_message>
Edit Test Data and start test by navigating to the home page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -1,87 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="29005"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/git/Selenium/noths-selenium-test/src/test/resources/testData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26580" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
-  <si>
-    <t>Test Case Name</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>abc@xyz.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>order_reference</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Customer service</t>
-  </si>
-  <si>
-    <t>abc@123.com</t>
-  </si>
-  <si>
-    <t>Testmessage1</t>
-  </si>
-  <si>
-    <t>Testmessage2</t>
-  </si>
-  <si>
-    <t>abc@234.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>bcd234</t>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>default_product</t>
+  </si>
+  <si>
+    <t>https://www.notonthehighstreet.com/</t>
+  </si>
+  <si>
+    <t>TD1</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>test_data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,14 +67,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,35 +96,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -214,12 +176,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -249,12 +211,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -458,112 +420,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
+      <c r="D2" s="2">
+        <v>318498</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -573,7 +474,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement the scenario PDP - Mainland UK Delivery Option
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Chrome</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>test_data</t>
+  </si>
+  <si>
+    <t>486442</t>
   </si>
 </sst>
 </file>
@@ -113,12 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +427,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -458,8 +462,8 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
-        <v>318498</v>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement the navigation to Mother's day gift page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Chrome</t>
   </si>
@@ -39,9 +39,6 @@
     <t>default_product</t>
   </si>
   <si>
-    <t>https://www.notonthehighstreet.com/</t>
-  </si>
-  <si>
     <t>TD1</t>
   </si>
   <si>
@@ -52,13 +49,22 @@
   </si>
   <si>
     <t>486442</t>
+  </si>
+  <si>
+    <t>/mothers-day/best-mothers-day-gifts</t>
+  </si>
+  <si>
+    <t>https://www.notonthehighstreet.com</t>
+  </si>
+  <si>
+    <t>mothers_day_gifts_path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +76,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,18 +127,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -436,39 +453,49 @@
     <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>